<commit_message>
Cambios al procesamiento de la cuenta de energía
</commit_message>
<xml_diff>
--- a/salidas/CIEE_2013_2020.xlsx
+++ b/salidas/CIEE_2013_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renato\GitHub\scn_scae_gt\salidas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D739107-035C-4A9F-A0FC-F22EFC944067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5041ADB-EE0E-42F3-B9F4-E1C31F27ED42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="712" yWindow="-98" windowWidth="18586" windowHeight="10996" xr2:uid="{7A45CCBD-7F7D-4E9D-B9DF-5CC6411513E8}"/>
   </bookViews>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB8DEAE-61F9-44C6-AA36-9D15DF2312E6}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -2618,7 +2618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE62E982-B27C-4270-8F0D-1C1D9F8C0329}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4344,7 +4344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15784741-4614-4986-BEFF-4FDF7A35EBB4}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -6070,7 +6070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A347FB0-058B-45D9-AC34-762D34EAE6B8}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7796,7 +7796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27347EEF-EB30-482E-97BD-D4EC99E0DC91}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -9522,7 +9522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F224B359-5033-4839-9386-9FAB43549EFC}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -11248,7 +11248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F04CD40-8ED9-43D4-9EC6-8FF1C1BFE828}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -12974,7 +12974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7883A72-4063-4836-A89C-8FE42D8112A7}">
   <dimension ref="B1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>